<commit_message>
writes and validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/project-metadata-steelhead.xlsx
+++ b/data-raw/metadata/project-metadata-steelhead.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/stanislaus-steelhead/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FAA373-E30D-D24A-86CA-BA3D1D08C06A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDB83B4-6AAD-0E42-AD61-8A50EE6CBBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -312,7 +312,7 @@
     <t>annually</t>
   </si>
   <si>
-    <t>Grant award to continue the Annual Monitoring and Reporting of Stanislaus River Steelhead Spawning. Award number R20AC00120-0.</t>
+    <t>R20AC00120-0</t>
   </si>
   <si>
     <t>U.S. Department of the Interior</t>
@@ -1240,7 +1240,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="A2:E3"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1295,6 +1295,14 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="114.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1320,12 +1328,11 @@
       <c r="A2" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" s="13" t="s">
+        <v>92</v>
+      </c>
       <c r="D2" t="s">
         <v>59</v>
-      </c>
-      <c r="F2" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates files for preview
</commit_message>
<xml_diff>
--- a/data-raw/metadata/project-metadata-steelhead.xlsx
+++ b/data-raw/metadata/project-metadata-steelhead.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/stanislaus-steelhead/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDB83B4-6AAD-0E42-AD61-8A50EE6CBBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B97FAD2-A1D6-EC4E-991B-C3C845B160E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="11" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="95">
   <si>
     <t>first_name</t>
   </si>
@@ -315,7 +315,10 @@
     <t>R20AC00120-0</t>
   </si>
   <si>
-    <t>U.S. Department of the Interior</t>
+    <t>U.S. Department of the Interior: Grant award to continue the Annual Monitoring and Reporting of Stanislaus River Steelhead Spawning</t>
+  </si>
+  <si>
+    <t>CVPIA</t>
   </si>
 </sst>
 </file>
@@ -1155,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1183,6 +1186,11 @@
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1290,13 +1298,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4676C8CC-00B2-CF46-8026-AD8CA8201F40}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
@@ -1391,8 +1399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1433,7 +1441,7 @@
         <v>49</v>
       </c>
       <c r="B2" s="2">
-        <v>120.939537</v>
+        <v>-120.939537</v>
       </c>
       <c r="C2" s="2">
         <v>-120.63265</v>

</xml_diff>